<commit_message>
GENESIS-23432423 ewrwe fw Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/npeError(2)(1)(4)/npeError(2)(1)(4).xlsx
+++ b/npeError(2)(1)(4)/npeError(2)(1)(4).xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="87">
   <si>
     <t>C1</t>
   </si>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>,test</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>(%a)</t>
+  </si>
+  <si>
+    <t>(&amp;a)</t>
+  </si>
+  <si>
+    <t>(&amp;b)</t>
   </si>
 </sst>
 </file>
@@ -692,428 +704,95 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7"/>
       <c r="E4" s="6"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14">
-      <c r="B14" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C16" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19">
-      <c r="B19" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21">
-      <c r="B21" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C23" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26">
-      <c r="B26" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="s" s="1">
-        <v>41</v>
-      </c>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28">
-      <c r="B28" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C30" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33">
-      <c r="B33" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35">
-      <c r="B35" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C37" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40">
-      <c r="B40" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42">
-      <c r="B42" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C44" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47">
-      <c r="B47" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49">
-      <c r="B49" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C49" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C50" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C51" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54">
-      <c r="B54" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C54" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56">
-      <c r="B56" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C56" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C57" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C58" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61">
-      <c r="B61" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C61" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63">
-      <c r="B63" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C63" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C64" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C65" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
     <row r="67">
       <c r="B67" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68">
       <c r="B68" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C68" t="s" s="1">
+      <c r="C68" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D68" t="s" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C69" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="1"/>
     </row>
     <row r="70">
       <c r="B70" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="C70" t="s" s="1">
+      <c r="C70" s="1"/>
+      <c r="D70" t="s" s="1">
         <v>65</v>
       </c>
     </row>
@@ -1121,7 +800,8 @@
       <c r="B71" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="C71" t="s" s="1">
+      <c r="C71" s="1"/>
+      <c r="D71" t="s" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1129,157 +809,32 @@
       <c r="B72" t="n" s="2">
         <v>1.0</v>
       </c>
-      <c r="C72" t="s" s="1">
+      <c r="C72" s="1"/>
+      <c r="D72" t="s" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="74">
-      <c r="B74" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C74" s="3"/>
-    </row>
-    <row r="75">
-      <c r="B75" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C75" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77">
-      <c r="B77" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C77" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C78" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C79" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C81" s="3"/>
-    </row>
-    <row r="82">
-      <c r="B82" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C82" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="B83" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84">
-      <c r="B84" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C84" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="B85" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C85" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="B86" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C86" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="B88" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C88" s="3"/>
-    </row>
-    <row r="89">
-      <c r="B89" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C89" t="s" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="B90" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91">
-      <c r="B91" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C91" t="s" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="B92" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="C92" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="B93" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C93" t="s" s="1">
-        <v>66</v>
-      </c>
-    </row>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B67:D67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>